<commit_message>
Implemented predators into MAIN sim
</commit_message>
<xml_diff>
--- a/predatorPrey_SPEED_TESTS.xlsx
+++ b/predatorPrey_SPEED_TESTS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\Documents\GitHub\ALife-Honours\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>TEST 1</t>
   </si>
@@ -101,10 +101,16 @@
     <t>Test 2 time was jummping up and down between 95ms-320ms. MOVE function consumes the most time in all tests.</t>
   </si>
   <si>
-    <t>BEFORE REFACTORING</t>
-  </si>
-  <si>
-    <t>AFTER REFACTORING</t>
+    <t>BEFORE ADDING PREDATORS</t>
+  </si>
+  <si>
+    <t>SECOND ROUND</t>
+  </si>
+  <si>
+    <t>FIRST ROUND</t>
+  </si>
+  <si>
+    <t>AFTER ADDING PREDATORS</t>
   </si>
 </sst>
 </file>
@@ -542,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G30"/>
+  <dimension ref="B1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,6 +562,11 @@
     <col min="7" max="7" width="39.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>25</v>
@@ -732,118 +743,126 @@
         <v>24</v>
       </c>
     </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="4"/>
+    </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>3</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C29" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
+      <c r="G29" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>